<commit_message>
Updated Drools rules with addTag privilege.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMILLE~1.ARM\ONEDRI~2\DOCUME~1\MobaXterm\slash\RemoteFiles\4\armdev@devvm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ArkCase\ACM3\acm-services\acm-service-data-access-control\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
   <si>
     <t>RuleSet</t>
   </si>
@@ -325,6 +325,33 @@
   </si>
   <si>
     <t>Task – Only participants can version files</t>
+  </si>
+  <si>
+    <t>Case File – Participants cannot version files</t>
+  </si>
+  <si>
+    <t>Task – Participants cannot version files</t>
+  </si>
+  <si>
+    <t>Complaint – Participants cannot upload or replace files</t>
+  </si>
+  <si>
+    <t>status != 'CLOSED' &amp;&amp; status != 'DELETE' &amp;&amp; status != 'DELETED'</t>
+  </si>
+  <si>
+    <t>status == 'CLOSED' || status == 'DELETE' || status == 'DELETED'</t>
+  </si>
+  <si>
+    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader, *</t>
+  </si>
+  <si>
+    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, *</t>
+  </si>
+  <si>
+    <t>Task – Only participants can add tags</t>
+  </si>
+  <si>
+    <t>grant addTag to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
   </si>
 </sst>
 </file>
@@ -558,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -591,6 +618,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,6 +782,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -787,6 +834,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -942,10 +1006,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G52"/>
+  <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,32 +1329,36 @@
       <c r="C26" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="17"/>
+      <c r="D26" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="17"/>
+      <c r="D27" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>31</v>
@@ -1299,92 +1367,92 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>45</v>
+        <v>79</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G29" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="D30" s="17"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G30" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="18" t="s">
-        <v>35</v>
+      <c r="G31" s="16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="17"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="16" t="s">
-        <v>41</v>
+      <c r="G33" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>45</v>
@@ -1393,50 +1461,48 @@
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="17" t="s">
-        <v>53</v>
-      </c>
+      <c r="D35" s="17"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
-      <c r="G36" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>56</v>
@@ -1447,25 +1513,27 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="17"/>
+      <c r="D38" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
-      <c r="G38" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G38" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>45</v>
@@ -1474,13 +1542,13 @@
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>45</v>
@@ -1489,88 +1557,92 @@
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="16" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="17"/>
+      <c r="D41" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="17"/>
+      <c r="D42" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="D43" s="17"/>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
-      <c r="G43" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G43" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="17"/>
+      <c r="D45" s="18"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
-      <c r="G45" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G45" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>60</v>
@@ -1579,13 +1651,13 @@
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="16" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>60</v>
@@ -1594,13 +1666,13 @@
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
       <c r="G47" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="16" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>60</v>
@@ -1609,13 +1681,13 @@
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>60</v>
@@ -1624,57 +1696,121 @@
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="17"/>
+      <c r="D50" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
       <c r="G50" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
-      <c r="G51" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D52" s="17"/>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
-      <c r="G52" s="18" t="s">
+      <c r="G52" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="17"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="17"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added grant addTag to * privilege for Case and Complaint.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ArkCase\ACM3\acm-services\acm-service-data-access-control\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="107">
   <si>
     <t>RuleSet</t>
   </si>
@@ -352,6 +352,15 @@
   </si>
   <si>
     <t>grant addTag to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>Complaint – Anybody can add tag</t>
+  </si>
+  <si>
+    <t>grant addTag to *</t>
+  </si>
+  <si>
+    <t>Case File – anyone can add tag</t>
   </si>
 </sst>
 </file>
@@ -1006,10 +1015,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G56"/>
+  <dimension ref="A2:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,86 +1397,86 @@
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>45</v>
+        <v>104</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G30" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="D31" s="17"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G31" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="18" t="s">
-        <v>35</v>
+      <c r="G32" s="16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="18"/>
+      <c r="D33" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="17"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
-      <c r="G34" s="16" t="s">
-        <v>41</v>
+      <c r="G34" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>45</v>
@@ -1476,50 +1485,48 @@
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>53</v>
-      </c>
+      <c r="D36" s="17"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
-      <c r="G37" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>56</v>
@@ -1530,25 +1537,27 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="17"/>
+      <c r="D39" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
-      <c r="G39" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G39" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>45</v>
@@ -1557,62 +1566,62 @@
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="20" t="s">
-        <v>98</v>
-      </c>
+      <c r="D41" s="17"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="17"/>
+      <c r="D43" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>45</v>
@@ -1621,58 +1630,58 @@
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="D45" s="17"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
-      <c r="G45" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G45" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="17"/>
+      <c r="D47" s="18"/>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
-      <c r="G47" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G47" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>60</v>
@@ -1681,13 +1690,13 @@
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="16" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>60</v>
@@ -1696,77 +1705,77 @@
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="16" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="20" t="s">
-        <v>98</v>
-      </c>
+      <c r="D50" s="17"/>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
       <c r="G50" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="20" t="s">
-        <v>99</v>
-      </c>
+      <c r="D51" s="17"/>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
       <c r="G51" s="16" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="17"/>
+      <c r="D52" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
       <c r="G52" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="16" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D53" s="17"/>
+      <c r="D53" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
       <c r="G53" s="16" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="16" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>60</v>
@@ -1775,36 +1784,66 @@
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="16" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="16" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D55" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D55" s="17"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
-      <c r="G55" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="16" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D56" s="17"/>
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
-      <c r="G56" s="18" t="s">
+      <c r="G56" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AFDP-3348: Configuration changes for new Document Repository module
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadica.cuculova\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="110">
   <si>
     <t>RuleSet</t>
   </si>
@@ -361,6 +361,15 @@
   </si>
   <si>
     <t>Case File – anyone can add tag</t>
+  </si>
+  <si>
+    <t>Document Repository-default read access</t>
+  </si>
+  <si>
+    <t>DOC_REPO</t>
+  </si>
+  <si>
+    <t>grant read to assignee, co-owner, supervisor, owning group, approver, collaborator, follower, reader, *</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1024,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G58"/>
+  <dimension ref="A2:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,6 +1854,21 @@
       <c r="F58" s="18"/>
       <c r="G58" s="18" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="16" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFDP-3349: - Add new access control rules for DocumentRepository - Add new events for DocumentRepository - Add module privilege for DocumentRepository - Add new facet field - Add new module for dashboard configuration
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="118">
   <si>
     <t>RuleSet</t>
   </si>
@@ -363,13 +363,37 @@
     <t>Case File – anyone can add tag</t>
   </si>
   <si>
-    <t>Document Repository-default read access</t>
-  </si>
-  <si>
     <t>DOC_REPO</t>
   </si>
   <si>
     <t>grant read to assignee, co-owner, supervisor, owning group, approver, collaborator, follower, reader, *</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Anybody can add comments</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Anybody can add tag</t>
+  </si>
+  <si>
+    <t>Document Repository -default read access</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Anybody can subscribe</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Restricted Flag</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Only participants can add files</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Only participants can save</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Only participants can upload or replace files</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1048,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G59"/>
+  <dimension ref="A2:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,16 +1883,130 @@
     <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" s="18" t="s">
         <v>107</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>108</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18"/>
       <c r="G59" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B60" s="16" t="s">
         <v>109</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B61" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B64" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B65" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D65" s="17"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B66" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D66" s="17"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B67" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFDP-3458: Add new MyDocuments module - Add views privileges for new module - Add creator ass default assignee for PERSONAL repositories - Deny read access to * participant
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadica.cuculova\.arkcase\acm\rules\"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="121">
   <si>
     <t>RuleSet</t>
   </si>
@@ -394,6 +394,15 @@
   </si>
   <si>
     <t>DocumentRepository – Only participants can upload or replace files</t>
+  </si>
+  <si>
+    <t>Document Repository -deny read access</t>
+  </si>
+  <si>
+    <t>repositoryType == 'PERSONAL'</t>
+  </si>
+  <si>
+    <t>mandatory deny read to *</t>
   </si>
 </sst>
 </file>
@@ -1048,10 +1057,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G67"/>
+  <dimension ref="A2:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1895,23 +1904,25 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B61" s="16" t="s">
         <v>109</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B61" s="16" t="s">
-        <v>110</v>
       </c>
       <c r="C61" s="16" t="s">
         <v>107</v>
@@ -1920,12 +1931,12 @@
       <c r="E61" s="16"/>
       <c r="F61" s="16"/>
       <c r="G61" s="16" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C62" s="16" t="s">
         <v>107</v>
@@ -1934,12 +1945,12 @@
       <c r="E62" s="16"/>
       <c r="F62" s="16"/>
       <c r="G62" s="16" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C63" s="16" t="s">
         <v>107</v>
@@ -1948,42 +1959,42 @@
       <c r="E63" s="16"/>
       <c r="F63" s="16"/>
       <c r="G63" s="16" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B65" s="16" t="s">
         <v>114</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B65" s="16" t="s">
-        <v>115</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D65" s="17"/>
+      <c r="D65" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="E65" s="18"/>
       <c r="F65" s="18"/>
-      <c r="G65" s="16" t="s">
-        <v>41</v>
+      <c r="G65" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C66" s="18" t="s">
         <v>107</v>
@@ -1992,20 +2003,34 @@
       <c r="E66" s="18"/>
       <c r="F66" s="18"/>
       <c r="G66" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C67" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D67" s="20"/>
+      <c r="D67" s="17"/>
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
       <c r="G67" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B68" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D68" s="20"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="16" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AFDP-3899 Contacts Management – Organization - Organization ACL
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadica.cuculova\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bojan.milenkoski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="169"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7320" tabRatio="169"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="128">
   <si>
     <t>RuleSet</t>
   </si>
@@ -403,6 +403,27 @@
   </si>
   <si>
     <t>mandatory deny read to *</t>
+  </si>
+  <si>
+    <t>ORGANIZATION</t>
+  </si>
+  <si>
+    <t>Organization – default read access</t>
+  </si>
+  <si>
+    <t>Organization – Only participants can save</t>
+  </si>
+  <si>
+    <t>Organization – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>grant save to owner, owning group, collaborator</t>
+  </si>
+  <si>
+    <t>grant read to owner, owning group, collaborator, reader, *</t>
+  </si>
+  <si>
+    <t>Organization – Restricted Flag</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1078,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G68"/>
+  <dimension ref="A2:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,6 +2053,64 @@
       <c r="F68" s="18"/>
       <c r="G68" s="16" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D69" s="17"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B70" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D70" s="17"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B71" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" s="17"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B72" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFDP-3892 Contacts Management – People - People ACL
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="133">
   <si>
     <t>RuleSet</t>
   </si>
@@ -424,6 +424,21 @@
   </si>
   <si>
     <t>Organization – Restricted Flag</t>
+  </si>
+  <si>
+    <t>PERSON</t>
+  </si>
+  <si>
+    <t>Person – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>Person – default read access</t>
+  </si>
+  <si>
+    <t>Person – Only participants can save</t>
+  </si>
+  <si>
+    <t>Person – Restricted Flag</t>
   </si>
 </sst>
 </file>
@@ -1078,10 +1093,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G72"/>
+  <dimension ref="A2:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,6 +2125,64 @@
       <c r="E72" s="18"/>
       <c r="F72" s="18"/>
       <c r="G72" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B73" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D73" s="17"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B74" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D74" s="17"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B75" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D75" s="17"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AFDP-4158 Document Level - ACL Implementation
File/Folder ACLs
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="142">
   <si>
     <t>RuleSet</t>
   </si>
@@ -240,15 +240,9 @@
     <t>grant delete to assignee, supervisor</t>
   </si>
   <si>
-    <t>Folder – default public access</t>
-  </si>
-  <si>
     <t>FOLDER</t>
   </si>
   <si>
-    <t>Folder –deny no access</t>
-  </si>
-  <si>
     <t>Object Types</t>
   </si>
   <si>
@@ -439,6 +433,39 @@
   </si>
   <si>
     <t>Person – Restricted Flag</t>
+  </si>
+  <si>
+    <t>Folder – deny no access</t>
+  </si>
+  <si>
+    <t>grant read to group-write, group-read, write, read, *</t>
+  </si>
+  <si>
+    <t>mandatory deny read to no-access, group-no-access</t>
+  </si>
+  <si>
+    <t>Folder – Restricted Flag</t>
+  </si>
+  <si>
+    <t>Folder - write to folder</t>
+  </si>
+  <si>
+    <t>grant write to group-write, write</t>
+  </si>
+  <si>
+    <t>Folder - default list folder</t>
+  </si>
+  <si>
+    <t>File - default read file</t>
+  </si>
+  <si>
+    <t>File - write</t>
+  </si>
+  <si>
+    <t>File – deny no access</t>
+  </si>
+  <si>
+    <t>File – Restricted Flag</t>
   </si>
 </sst>
 </file>
@@ -1093,10 +1120,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G76"/>
+  <dimension ref="A2:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,41 +1438,41 @@
     <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>31</v>
@@ -1454,13 +1481,13 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>31</v>
@@ -1469,13 +1496,13 @@
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>31</v>
@@ -1484,7 +1511,7 @@
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1635,7 +1662,7 @@
     <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>45</v>
@@ -1644,7 +1671,7 @@
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1659,47 +1686,47 @@
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>45</v>
@@ -1708,13 +1735,13 @@
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>45</v>
@@ -1723,13 +1750,13 @@
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>45</v>
@@ -1738,7 +1765,7 @@
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1804,7 +1831,7 @@
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>60</v>
@@ -1819,41 +1846,41 @@
     <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>60</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
       <c r="G52" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>60</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
       <c r="G53" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>60</v>
@@ -1862,13 +1889,13 @@
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>60</v>
@@ -1877,13 +1904,13 @@
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
       <c r="G55" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>60</v>
@@ -1892,297 +1919,391 @@
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
       <c r="G56" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>67</v>
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
-      <c r="G57" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="16" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
       <c r="F58" s="18"/>
-      <c r="G58" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G58" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="16" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18"/>
       <c r="G59" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
       <c r="B60" s="16" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
-      <c r="G60" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G60" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
       <c r="B61" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
+        <v>138</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
       <c r="G61" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
       <c r="B62" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C62" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B63" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16" t="s">
+      <c r="C65" s="18" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B64" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B65" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>56</v>
-      </c>
+      <c r="D65" s="18"/>
       <c r="E65" s="18"/>
       <c r="F65" s="18"/>
-      <c r="G65" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G65" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D66" s="17"/>
+        <v>105</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>117</v>
+      </c>
       <c r="E66" s="18"/>
       <c r="F66" s="18"/>
       <c r="G66" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C67" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D67" s="17"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
+      <c r="C67" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
       <c r="G67" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D68" s="20"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
+        <v>108</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
       <c r="G68" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="D69" s="17"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="D70" s="17"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
+        <v>111</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
       <c r="G70" s="16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="D71" s="17"/>
+        <v>112</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="E71" s="18"/>
       <c r="F71" s="18"/>
-      <c r="G71" s="16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G71" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>56</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D72" s="17"/>
       <c r="E72" s="18"/>
       <c r="F72" s="18"/>
-      <c r="G72" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G72" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B73" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>128</v>
+        <v>114</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>105</v>
       </c>
       <c r="D73" s="17"/>
       <c r="E73" s="18"/>
       <c r="F73" s="18"/>
-      <c r="G73" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G73" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B74" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D74" s="17"/>
+        <v>115</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D74" s="20"/>
       <c r="E74" s="18"/>
       <c r="F74" s="18"/>
       <c r="G74" s="16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B75" s="16" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D75" s="17"/>
       <c r="E75" s="18"/>
       <c r="F75" s="18"/>
-      <c r="G75" s="16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G75" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D76" s="18" t="s">
-        <v>56</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="D76" s="17"/>
       <c r="E76" s="18"/>
       <c r="F76" s="18"/>
-      <c r="G76" s="18" t="s">
+      <c r="G76" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B77" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D77" s="17"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B78" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D79" s="17"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B80" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D80" s="17"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B81" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D81" s="17"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2212,10 +2333,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2223,7 +2344,7 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2231,22 +2352,22 @@
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added: - Costsheet – default read access, Costsheet – Only participants can add files, Costsheet – Only participants can save and Costsheet –  Only participants can upload or replace files in drools-access-control-rules.xlsx - Costsheet – Default access, Costsheet - creator read access and Costsheet – Default owner in drools-assignment-rules.xlsx
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjan.trifunov\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana.shekerova\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D891C9-625A-49BD-B74C-93C67608C5F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,8 +21,13 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="179021" calcMode="manual" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="146">
   <si>
     <t>RuleSet</t>
   </si>
@@ -460,11 +466,35 @@
   <si>
     <t>grant uploadOrReplaceFile to  owner, owning group, collaborator, *</t>
   </si>
+  <si>
+    <t>Costsheet – Only participants can add files</t>
+  </si>
+  <si>
+    <t>COSTSHEET</t>
+  </si>
+  <si>
+    <t>grant add file to assignee, owner, co-owner, supervisor, owning group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>Costsheet – default read access</t>
+  </si>
+  <si>
+    <t>Costsheet – Only participants can save</t>
+  </si>
+  <si>
+    <t>grant save to assignee, owner, co-owner, supervisor, owning group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, owner, co-owner, supervisor, owning group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>Costsheet –  Only participants can upload or replace files</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
@@ -1109,29 +1139,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G81"/>
+  <dimension ref="A2:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C57" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="49.85546875" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1"/>
-    <col min="8" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="3" max="3" width="49.81640625" customWidth="1"/>
+    <col min="4" max="4" width="36.1796875" customWidth="1"/>
+    <col min="5" max="5" width="43.81640625" customWidth="1"/>
+    <col min="6" max="6" width="30.54296875" customWidth="1"/>
+    <col min="7" max="7" width="35.54296875" customWidth="1"/>
+    <col min="8" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1141,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -1151,7 +1181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1161,7 +1191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1171,7 +1201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1181,7 +1211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1191,7 +1221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1201,7 +1231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1211,7 +1241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1221,7 +1251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1231,7 +1261,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="348" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1241,7 +1271,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
@@ -1251,7 +1281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -1262,7 +1292,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1281,7 +1311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="4" t="s">
@@ -1292,7 +1322,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
@@ -1311,7 +1341,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
@@ -1334,7 +1364,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="16" t="s">
         <v>30</v>
@@ -1349,7 +1379,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="16" t="s">
         <v>33</v>
@@ -1366,7 +1396,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
@@ -1383,7 +1413,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="16" t="s">
         <v>38</v>
@@ -1398,7 +1428,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
@@ -1413,7 +1443,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="16" t="s">
         <v>42</v>
@@ -1428,7 +1458,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="16" t="s">
         <v>44</v>
@@ -1445,7 +1475,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
         <v>47</v>
@@ -1462,7 +1492,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
         <v>50</v>
@@ -1477,7 +1507,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
         <v>52</v>
@@ -1492,7 +1522,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
         <v>54</v>
@@ -1507,7 +1537,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
         <v>56</v>
@@ -1522,7 +1552,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
         <v>58</v>
@@ -1539,7 +1569,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
         <v>60</v>
@@ -1556,7 +1586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
         <v>61</v>
@@ -1571,7 +1601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
         <v>62</v>
@@ -1586,7 +1616,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
         <v>63</v>
@@ -1601,7 +1631,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
         <v>64</v>
@@ -1618,7 +1648,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
         <v>67</v>
@@ -1635,7 +1665,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
         <v>70</v>
@@ -1652,7 +1682,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
         <v>71</v>
@@ -1667,7 +1697,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
         <v>63</v>
@@ -1682,7 +1712,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
         <v>74</v>
@@ -1699,7 +1729,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
         <v>76</v>
@@ -1716,7 +1746,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
         <v>77</v>
@@ -1731,7 +1761,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
         <v>79</v>
@@ -1746,7 +1776,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
         <v>80</v>
@@ -1761,7 +1791,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="16" t="s">
         <v>81</v>
@@ -1776,7 +1806,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="16" t="s">
         <v>83</v>
@@ -1791,7 +1821,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="16" t="s">
         <v>84</v>
@@ -1806,7 +1836,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="16" t="s">
         <v>85</v>
@@ -1821,7 +1851,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
         <v>87</v>
@@ -1836,7 +1866,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
         <v>89</v>
@@ -1853,7 +1883,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="16" t="s">
         <v>90</v>
@@ -1870,7 +1900,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="16" t="s">
         <v>91</v>
@@ -1885,7 +1915,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="16" t="s">
         <v>92</v>
@@ -1900,7 +1930,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="16" t="s">
         <v>94</v>
@@ -1915,7 +1945,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="16" t="s">
         <v>96</v>
@@ -1930,7 +1960,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="16" t="s">
         <v>99</v>
@@ -1945,7 +1975,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="16" t="s">
         <v>101</v>
@@ -1960,7 +1990,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="16" t="s">
         <v>103</v>
@@ -1977,7 +2007,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="B61" s="16" t="s">
         <v>104</v>
@@ -1992,7 +2022,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="16" t="s">
         <v>106</v>
@@ -2007,7 +2037,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="16" t="s">
         <v>107</v>
@@ -2022,7 +2052,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="16" t="s">
         <v>108</v>
@@ -2039,7 +2069,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="16" t="s">
         <v>109</v>
@@ -2054,7 +2084,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B66" s="16" t="s">
         <v>111</v>
       </c>
@@ -2068,7 +2098,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B67" s="16" t="s">
         <v>112</v>
       </c>
@@ -2082,7 +2112,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B68" s="16" t="s">
         <v>113</v>
       </c>
@@ -2096,7 +2126,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B69" s="16" t="s">
         <v>114</v>
       </c>
@@ -2110,7 +2140,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B70" s="16" t="s">
         <v>115</v>
       </c>
@@ -2126,7 +2156,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B71" s="16" t="s">
         <v>116</v>
       </c>
@@ -2140,7 +2170,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B72" s="16" t="s">
         <v>116</v>
       </c>
@@ -2154,7 +2184,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B73" s="16" t="s">
         <v>117</v>
       </c>
@@ -2168,7 +2198,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B74" s="16" t="s">
         <v>118</v>
       </c>
@@ -2182,7 +2212,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B75" s="16" t="s">
         <v>120</v>
       </c>
@@ -2196,7 +2226,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B76" s="16" t="s">
         <v>122</v>
       </c>
@@ -2210,7 +2240,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B77" s="16" t="s">
         <v>124</v>
       </c>
@@ -2226,7 +2256,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B78" s="16" t="s">
         <v>125</v>
       </c>
@@ -2240,7 +2270,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B79" s="16" t="s">
         <v>127</v>
       </c>
@@ -2254,7 +2284,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B80" s="16" t="s">
         <v>128</v>
       </c>
@@ -2268,7 +2298,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B81" s="16" t="s">
         <v>129</v>
       </c>
@@ -2284,14 +2314,74 @@
         <v>69</v>
       </c>
     </row>
+    <row r="82" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="1"/>
+      <c r="B82" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1"/>
+      <c r="B83" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D83" s="17"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="1"/>
+      <c r="B84" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D84" s="17"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="1"/>
+      <c r="B85" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D85" s="20"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -2301,14 +2391,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>130</v>
       </c>
@@ -2316,7 +2406,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2324,7 +2414,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -2332,17 +2422,17 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -2354,7 +2444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -2362,9 +2452,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
AFDP-7048 - Global New Task and New Task from the Document Tree - Modal changes
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana.shekerova\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefan.sanevski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D891C9-625A-49BD-B74C-93C67608C5F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{938CCBCF-9D08-4FB9-A81E-040984CE17FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,13 +21,8 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="179021" calcMode="manual" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" calcMode="manual" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -36,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="148">
   <si>
     <t>RuleSet</t>
   </si>
@@ -489,6 +484,12 @@
   </si>
   <si>
     <t>Costsheet –  Only participants can upload or replace files</t>
+  </si>
+  <si>
+    <t>BUSINESS_PROCESS</t>
+  </si>
+  <si>
+    <t>BusinessProcess – Grant Access</t>
   </si>
 </sst>
 </file>
@@ -1143,25 +1144,25 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G85"/>
+  <dimension ref="A2:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
-    <col min="3" max="3" width="49.81640625" customWidth="1"/>
-    <col min="4" max="4" width="36.1796875" customWidth="1"/>
-    <col min="5" max="5" width="43.81640625" customWidth="1"/>
-    <col min="6" max="6" width="30.54296875" customWidth="1"/>
-    <col min="7" max="7" width="35.54296875" customWidth="1"/>
-    <col min="8" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="8" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1171,7 +1172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -1181,7 +1182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1191,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1201,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1211,7 +1212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1221,7 +1222,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1231,7 +1232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1241,7 +1242,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1251,7 +1252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1261,7 +1262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="348" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="360" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1271,7 +1272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
@@ -1281,7 +1282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -1292,7 +1293,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1311,7 +1312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="4" t="s">
@@ -1322,7 +1323,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
@@ -1341,7 +1342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
@@ -1364,7 +1365,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="16" t="s">
         <v>30</v>
@@ -1379,7 +1380,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="16" t="s">
         <v>33</v>
@@ -1396,7 +1397,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
@@ -1413,7 +1414,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="16" t="s">
         <v>38</v>
@@ -1428,7 +1429,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
@@ -1443,7 +1444,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="16" t="s">
         <v>42</v>
@@ -1458,7 +1459,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="16" t="s">
         <v>44</v>
@@ -1475,7 +1476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
         <v>47</v>
@@ -1492,7 +1493,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
         <v>50</v>
@@ -1507,7 +1508,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
         <v>52</v>
@@ -1522,7 +1523,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
         <v>54</v>
@@ -1537,7 +1538,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
         <v>56</v>
@@ -1552,7 +1553,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
         <v>58</v>
@@ -1569,7 +1570,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
         <v>60</v>
@@ -1586,7 +1587,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
         <v>61</v>
@@ -1601,7 +1602,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
         <v>62</v>
@@ -1616,7 +1617,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
         <v>63</v>
@@ -1631,7 +1632,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
         <v>64</v>
@@ -1648,7 +1649,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
         <v>67</v>
@@ -1665,7 +1666,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
         <v>70</v>
@@ -1682,7 +1683,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
         <v>71</v>
@@ -1697,7 +1698,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
         <v>63</v>
@@ -1712,7 +1713,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
         <v>74</v>
@@ -1729,7 +1730,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
         <v>76</v>
@@ -1746,7 +1747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
         <v>77</v>
@@ -1761,7 +1762,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
         <v>79</v>
@@ -1776,7 +1777,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
         <v>80</v>
@@ -1791,7 +1792,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="16" t="s">
         <v>81</v>
@@ -1806,7 +1807,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="16" t="s">
         <v>83</v>
@@ -1821,7 +1822,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="16" t="s">
         <v>84</v>
@@ -1836,7 +1837,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="16" t="s">
         <v>85</v>
@@ -1851,7 +1852,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
         <v>87</v>
@@ -1866,7 +1867,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
         <v>89</v>
@@ -1883,7 +1884,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="16" t="s">
         <v>90</v>
@@ -1900,7 +1901,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="16" t="s">
         <v>91</v>
@@ -1915,7 +1916,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="16" t="s">
         <v>92</v>
@@ -1930,7 +1931,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="16" t="s">
         <v>94</v>
@@ -1945,7 +1946,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="16" t="s">
         <v>96</v>
@@ -1960,7 +1961,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="16" t="s">
         <v>99</v>
@@ -1975,7 +1976,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="16" t="s">
         <v>101</v>
@@ -1990,7 +1991,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="16" t="s">
         <v>103</v>
@@ -2007,7 +2008,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="16" t="s">
         <v>104</v>
@@ -2022,7 +2023,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="16" t="s">
         <v>106</v>
@@ -2037,7 +2038,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="16" t="s">
         <v>107</v>
@@ -2052,7 +2053,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="16" t="s">
         <v>108</v>
@@ -2069,7 +2070,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="16" t="s">
         <v>109</v>
@@ -2084,7 +2085,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="16" t="s">
         <v>111</v>
       </c>
@@ -2098,7 +2099,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
         <v>112</v>
       </c>
@@ -2112,7 +2113,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="16" t="s">
         <v>113</v>
       </c>
@@ -2126,7 +2127,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="16" t="s">
         <v>114</v>
       </c>
@@ -2140,7 +2141,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="16" t="s">
         <v>115</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
         <v>116</v>
       </c>
@@ -2170,7 +2171,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
         <v>116</v>
       </c>
@@ -2184,7 +2185,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" s="16" t="s">
         <v>117</v>
       </c>
@@ -2198,7 +2199,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="16" t="s">
         <v>118</v>
       </c>
@@ -2212,7 +2213,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B75" s="16" t="s">
         <v>120</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
         <v>122</v>
       </c>
@@ -2240,7 +2241,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="16" t="s">
         <v>124</v>
       </c>
@@ -2256,7 +2257,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="16" t="s">
         <v>125</v>
       </c>
@@ -2270,7 +2271,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="16" t="s">
         <v>127</v>
       </c>
@@ -2284,7 +2285,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="16" t="s">
         <v>128</v>
       </c>
@@ -2298,7 +2299,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" s="16" t="s">
         <v>129</v>
       </c>
@@ -2314,7 +2315,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="16" t="s">
         <v>141</v>
@@ -2329,7 +2330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="16" t="s">
         <v>138</v>
@@ -2344,7 +2345,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="16" t="s">
         <v>142</v>
@@ -2359,7 +2360,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="16" t="s">
         <v>145</v>
@@ -2372,6 +2373,20 @@
       <c r="F85" s="18"/>
       <c r="G85" s="16" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B86" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D86" s="17"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2391,14 +2406,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>130</v>
       </c>
@@ -2406,7 +2421,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2414,7 +2429,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -2422,17 +2437,17 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -2452,9 +2467,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
AFDP-7623 CORE - Created new Participant Type - "Collaborator Group"
</commit_message>
<xml_diff>
--- a/acm/rules/drools-access-control-rules.xlsx
+++ b/acm/rules/drools-access-control-rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefan.sanevski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.serafimoska\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{938CCBCF-9D08-4FB9-A81E-040984CE17FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93396525-F525-4644-9FEB-777D82104CEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -171,33 +171,21 @@
     <t>Complaint – Only participants can add files</t>
   </si>
   <si>
-    <t>grant add file to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
     <t>Complaint – Only participants can save</t>
   </si>
   <si>
-    <t>grant save to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
     <t>Complaint – Everyone can upload or replace files</t>
   </si>
   <si>
     <t>status != 'CLOSED' &amp;&amp; status != 'DELETE' &amp;&amp; status != 'DELETED'</t>
   </si>
   <si>
-    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader, follower,  *</t>
-  </si>
-  <si>
     <t>Complaint – Deny upload or replace files on closed complaint</t>
   </si>
   <si>
     <t>status == 'CLOSED' || status == 'DELETE' || status == 'DELETED'</t>
   </si>
   <si>
-    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader, follower, *</t>
-  </si>
-  <si>
     <t>Complaint – Anybody can add comments</t>
   </si>
   <si>
@@ -225,9 +213,6 @@
     <t>Case File – Grant Participants Access to Drafts</t>
   </si>
   <si>
-    <t>grant read to assignee, co-owner, supervisor, owning group, approver, collaborator, follower, reader</t>
-  </si>
-  <si>
     <t>Case File – Grant Access to non-Drafts</t>
   </si>
   <si>
@@ -246,9 +231,6 @@
     <t>status == 'DELETED'</t>
   </si>
   <si>
-    <t>mandatory deny read to assignee, co-owner, supervisor, owning group, approver, collaborator, *</t>
-  </si>
-  <si>
     <t>Complaint – Restricted Flag</t>
   </si>
   <si>
@@ -264,27 +246,15 @@
     <t>Case File – Only participants can view details page</t>
   </si>
   <si>
-    <t>grant viewCaseDetailsPage to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
-  </si>
-  <si>
-    <t>grant saveCase to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
     <t>Case File – Everyone can upload or replace files</t>
   </si>
   <si>
-    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader, follower, *</t>
-  </si>
-  <si>
     <t>Case File –  Deny upload or replace files on closed case file</t>
   </si>
   <si>
     <t>Case File – Only participants can add comments</t>
   </si>
   <si>
-    <t>grant addComment to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
-  </si>
-  <si>
     <t>Case File – anyone can subscribe</t>
   </si>
   <si>
@@ -333,9 +303,6 @@
     <t>Task – Only participants can add tags</t>
   </si>
   <si>
-    <t>grant addTag to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
-  </si>
-  <si>
     <t>Folder - default list folder</t>
   </si>
   <si>
@@ -411,15 +378,9 @@
     <t>Organization – default read access</t>
   </si>
   <si>
-    <t>grant read to owner, owning group, collaborator, reader, *</t>
-  </si>
-  <si>
     <t>Organization – Only participants can save</t>
   </si>
   <si>
-    <t>grant save to owner, owning group, collaborator</t>
-  </si>
-  <si>
     <t>Organization – Restricted Flag</t>
   </si>
   <si>
@@ -456,33 +417,18 @@
     <t>ACCESS CONTROL LIST</t>
   </si>
   <si>
-    <t>grant add file to owner, owning group, collaborator, *</t>
-  </si>
-  <si>
-    <t>grant uploadOrReplaceFile to  owner, owning group, collaborator, *</t>
-  </si>
-  <si>
     <t>Costsheet – Only participants can add files</t>
   </si>
   <si>
     <t>COSTSHEET</t>
   </si>
   <si>
-    <t>grant add file to assignee, owner, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
     <t>Costsheet – default read access</t>
   </si>
   <si>
     <t>Costsheet – Only participants can save</t>
   </si>
   <si>
-    <t>grant save to assignee, owner, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
-    <t>grant uploadOrReplaceFile to assignee, owner, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
     <t>Costsheet –  Only participants can upload or replace files</t>
   </si>
   <si>
@@ -490,6 +436,60 @@
   </si>
   <si>
     <t>BusinessProcess – Grant Access</t>
+  </si>
+  <si>
+    <t>grant add file to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant save to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower,  *</t>
+  </si>
+  <si>
+    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower, *</t>
+  </si>
+  <si>
+    <t>grant read to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, follower, reader</t>
+  </si>
+  <si>
+    <t>mandatory deny read to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, *</t>
+  </si>
+  <si>
+    <t>grant viewCaseDetailsPage to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>grant saveCase to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower, *</t>
+  </si>
+  <si>
+    <t>grant addComment to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>grant addTag to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>grant read to owner, owning group, collaborator group, collaborator, reader, *</t>
+  </si>
+  <si>
+    <t>grant add file to owner, owning group, collaborator group, collaborator, *</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to  owner, owning group, collaborator group, collaborator, *</t>
+  </si>
+  <si>
+    <t>grant save to owner, owning group, collaborator group, collaborator</t>
+  </si>
+  <si>
+    <t>grant add file to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant save to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
   </si>
 </sst>
 </file>
@@ -1146,8 +1146,8 @@
   </sheetPr>
   <dimension ref="A2:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1429,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
@@ -1441,13 +1441,13 @@
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>31</v>
@@ -1456,47 +1456,47 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>31</v>
@@ -1505,13 +1505,13 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>31</v>
@@ -1520,13 +1520,13 @@
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>31</v>
@@ -1535,16 +1535,16 @@
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="18"/>
@@ -1553,13 +1553,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>34</v>
@@ -1567,16 +1567,16 @@
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="16" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>37</v>
@@ -1590,10 +1590,10 @@
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -1602,203 +1602,203 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="16" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="16" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D45" s="17"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="16" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
@@ -1807,304 +1807,304 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="16" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D48" s="17"/>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="16" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D49" s="17"/>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="16" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="16" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
       <c r="G50" s="16" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D51" s="17"/>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
       <c r="G51" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
       <c r="G52" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="16" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
       <c r="G53" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="16" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="16" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="16" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
       <c r="G55" s="16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="16" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D56" s="17"/>
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
       <c r="G56" s="16" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="16" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
       <c r="G57" s="16" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="16" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
       <c r="F58" s="18"/>
       <c r="G58" s="16" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="16" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18"/>
       <c r="G59" s="16" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="16" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
       <c r="G60" s="18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="16" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18"/>
       <c r="G61" s="16" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="16" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
       <c r="F62" s="18"/>
       <c r="G62" s="16" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="16" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
       <c r="G63" s="16" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="16" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
       <c r="G64" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="16" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
       <c r="F65" s="18"/>
       <c r="G65" s="16" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="16" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
       <c r="F66" s="16"/>
       <c r="G66" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
@@ -2115,96 +2115,96 @@
     </row>
     <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="16" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="16"/>
       <c r="F68" s="16"/>
       <c r="G68" s="16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="16" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
       <c r="F69" s="16"/>
       <c r="G69" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="16" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E70" s="18"/>
       <c r="F70" s="18"/>
       <c r="G70" s="18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D71" s="17"/>
       <c r="E71" s="18"/>
       <c r="F71" s="18"/>
       <c r="G71" s="16" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D72" s="17"/>
       <c r="E72" s="18"/>
       <c r="F72" s="18"/>
       <c r="G72" s="16" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" s="16" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D73" s="17"/>
       <c r="E73" s="18"/>
       <c r="F73" s="18"/>
       <c r="G73" s="16" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="16" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D74" s="17"/>
       <c r="E74" s="18"/>
@@ -2213,56 +2213,56 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B75" s="16" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D75" s="17"/>
       <c r="E75" s="18"/>
       <c r="F75" s="18"/>
       <c r="G75" s="16" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D76" s="17"/>
       <c r="E76" s="18"/>
       <c r="F76" s="18"/>
       <c r="G76" s="16" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="16" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E77" s="18"/>
       <c r="F77" s="18"/>
       <c r="G77" s="18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="16" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D78" s="17"/>
       <c r="E78" s="18"/>
@@ -2271,57 +2271,57 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B79" s="16" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D79" s="17"/>
       <c r="E79" s="18"/>
       <c r="F79" s="18"/>
       <c r="G79" s="16" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="16" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D80" s="17"/>
       <c r="E80" s="18"/>
       <c r="F80" s="18"/>
       <c r="G80" s="16" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" s="16" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E81" s="18"/>
       <c r="F81" s="18"/>
       <c r="G81" s="18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="16" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D82" s="18"/>
       <c r="E82" s="18"/>
@@ -2330,57 +2330,57 @@
         <v>35</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="16" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D83" s="17"/>
       <c r="E83" s="18"/>
       <c r="F83" s="18"/>
       <c r="G83" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="16" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D84" s="17"/>
       <c r="E84" s="18"/>
       <c r="F84" s="18"/>
       <c r="G84" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="16" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D85" s="20"/>
       <c r="E85" s="18"/>
       <c r="F85" s="18"/>
       <c r="G85" s="16" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B86" s="16" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="D86" s="17"/>
       <c r="E86" s="18"/>
@@ -2415,10 +2415,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2426,30 +2426,30 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>